<commit_message>
Adicionado upload de Excel
</commit_message>
<xml_diff>
--- a/Epo.Calculo.Web/Excel/Exemplo Importar Planilha - 3001.xlsx
+++ b/Epo.Calculo.Web/Excel/Exemplo Importar Planilha - 3001.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E105405\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12120"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>Data inicio</t>
   </si>
@@ -126,13 +121,35 @@
   </si>
   <si>
     <t>Numero</t>
+  </si>
+  <si>
+    <t>20.03.2019</t>
+  </si>
+  <si>
+    <t>20.03.2020</t>
+  </si>
+  <si>
+    <t>Flavio Henrique</t>
+  </si>
+  <si>
+    <t>03945000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,10 +196,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -190,9 +208,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -462,7 +484,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -470,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK3"/>
+  <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3:W3"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,7 +520,7 @@
     <col min="19" max="19" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.28515625" customWidth="1"/>
+    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="7.140625" bestFit="1" customWidth="1"/>
@@ -628,11 +650,11 @@
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>43544</v>
-      </c>
-      <c r="B2" s="2">
-        <v>43910</v>
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -702,11 +724,11 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>43544</v>
-      </c>
-      <c r="B3" s="2">
-        <v>43910</v>
+      <c r="A3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -754,10 +776,67 @@
         <v>1</v>
       </c>
       <c r="AE3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>1234567890</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4">
+        <v>277</v>
+      </c>
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="1">
+        <v>2019</v>
+      </c>
+      <c r="V4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="W4">
+        <v>10</v>
+      </c>
+      <c r="X4">
+        <v>100000</v>
+      </c>
+      <c r="Y4">
+        <v>40</v>
+      </c>
+      <c r="AB4">
+        <v>1</v>
+      </c>
+      <c r="AC4">
+        <v>100000</v>
+      </c>
+      <c r="AD4">
+        <v>1</v>
+      </c>
+      <c r="AE4">
         <v>100000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adicionado codificação de validação de campos do tipo data e logica para criação de campos dinamicos
</commit_message>
<xml_diff>
--- a/Epo.Calculo.Web/Excel/Exemplo Importar Planilha - 3001.xlsx
+++ b/Epo.Calculo.Web/Excel/Exemplo Importar Planilha - 3001.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>Data inicio</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>03945000</t>
+  </si>
+  <si>
+    <t>40/20/2020</t>
+  </si>
+  <si>
+    <t>10/20/2019</t>
   </si>
 </sst>
 </file>
@@ -484,7 +490,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -494,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,7 +657,7 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>35</v>
@@ -728,7 +734,7 @@
         <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Adicionado codificação para validar campos
</commit_message>
<xml_diff>
--- a/Epo.Calculo.Web/Excel/Exemplo Importar Planilha - 3001.xlsx
+++ b/Epo.Calculo.Web/Excel/Exemplo Importar Planilha - 3001.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
     <t>Data inicio</t>
   </si>
@@ -126,9 +126,6 @@
     <t>20.03.2019</t>
   </si>
   <si>
-    <t>20.03.2020</t>
-  </si>
-  <si>
     <t>Flavio Henrique</t>
   </si>
   <si>
@@ -139,6 +136,30 @@
   </si>
   <si>
     <t>10/20/2019</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>fa</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>hhh</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>kkkk</t>
+  </si>
+  <si>
+    <t>dsds</t>
+  </si>
+  <si>
+    <t>50.50.2020</t>
   </si>
 </sst>
 </file>
@@ -501,7 +522,7 @@
   <dimension ref="A1:AK4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,10 +678,10 @@
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>25</v>
@@ -677,9 +698,6 @@
       <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="L2">
-        <v>277</v>
-      </c>
       <c r="M2" t="s">
         <v>5</v>
       </c>
@@ -691,9 +709,6 @@
       </c>
       <c r="W2">
         <v>999</v>
-      </c>
-      <c r="X2">
-        <v>100000</v>
       </c>
       <c r="Y2">
         <v>20</v>
@@ -734,7 +749,7 @@
         <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
@@ -757,11 +772,9 @@
       <c r="M3" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="1">
-        <v>2019</v>
-      </c>
-      <c r="V3">
-        <v>1322000</v>
+      <c r="N3" s="1"/>
+      <c r="V3" t="s">
+        <v>44</v>
       </c>
       <c r="W3">
         <v>999</v>
@@ -769,14 +782,14 @@
       <c r="X3">
         <v>100000</v>
       </c>
-      <c r="Y3">
-        <v>20</v>
+      <c r="Y3" t="s">
+        <v>39</v>
       </c>
       <c r="AB3">
         <v>1</v>
       </c>
-      <c r="AC3">
-        <v>100000</v>
+      <c r="AC3" t="s">
+        <v>42</v>
       </c>
       <c r="AD3">
         <v>1</v>
@@ -790,16 +803,16 @@
         <v>34</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="D4">
-        <v>1234567890</v>
+      <c r="D4" t="s">
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -807,8 +820,8 @@
       <c r="G4" t="s">
         <v>24</v>
       </c>
-      <c r="L4">
-        <v>277</v>
+      <c r="L4" t="s">
+        <v>41</v>
       </c>
       <c r="M4" t="s">
         <v>24</v>
@@ -817,7 +830,7 @@
         <v>2019</v>
       </c>
       <c r="V4" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W4">
         <v>10</v>
@@ -828,8 +841,8 @@
       <c r="Y4">
         <v>40</v>
       </c>
-      <c r="AB4">
-        <v>1</v>
+      <c r="AB4" t="s">
+        <v>43</v>
       </c>
       <c r="AC4">
         <v>100000</v>

</xml_diff>

<commit_message>
Atualização logica de importar planilha excel
</commit_message>
<xml_diff>
--- a/Epo.Calculo.Web/Excel/Exemplo Importar Planilha - 3001.xlsx
+++ b/Epo.Calculo.Web/Excel/Exemplo Importar Planilha - 3001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12120"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="28800" windowHeight="12060"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="51">
   <si>
     <t>Data inicio</t>
   </si>
@@ -160,6 +160,18 @@
   </si>
   <si>
     <t>50.50.2020</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>100B000</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>1500A</t>
   </si>
 </sst>
 </file>
@@ -511,7 +523,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -521,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AF4" sqref="AF4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +567,7 @@
     <col min="29" max="29" width="7" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="7" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.5703125" customWidth="1"/>
     <col min="33" max="33" width="7" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="7" bestFit="1" customWidth="1"/>
@@ -725,8 +737,8 @@
       <c r="AE2">
         <v>100000</v>
       </c>
-      <c r="AF2">
-        <v>7</v>
+      <c r="AF2" t="s">
+        <v>47</v>
       </c>
       <c r="AG2">
         <v>100000</v>
@@ -734,8 +746,8 @@
       <c r="AH2">
         <v>11</v>
       </c>
-      <c r="AI2">
-        <v>100000</v>
+      <c r="AI2" t="s">
+        <v>48</v>
       </c>
       <c r="AJ2">
         <v>15</v>
@@ -852,6 +864,12 @@
       </c>
       <c r="AE4">
         <v>100000</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>